<commit_message>
Have some more data, including a starter JSON file. Also added a starter index.html and JavaScript file
</commit_message>
<xml_diff>
--- a/map-data.xlsx
+++ b/map-data.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\development\map-challenge\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\map-challenge\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11990"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Asia</t>
   </si>
@@ -93,6 +93,51 @@
   </si>
   <si>
     <t>https://en.wikipedia.org/wiki/List_of_sovereign_states_and_dependent_territories_in_Asia</t>
+  </si>
+  <si>
+    <t>Cambodia</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>Kabul</t>
+  </si>
+  <si>
+    <t>Yerevan</t>
+  </si>
+  <si>
+    <t>Baku</t>
+  </si>
+  <si>
+    <t>Manama</t>
+  </si>
+  <si>
+    <t>Dhaka</t>
+  </si>
+  <si>
+    <t>Thimphu</t>
+  </si>
+  <si>
+    <t>Bandar Seri Begawan</t>
+  </si>
+  <si>
+    <t>Phnom Penh</t>
+  </si>
+  <si>
+    <t>Beijing</t>
+  </si>
+  <si>
+    <t>Yangtze</t>
+  </si>
+  <si>
+    <t>Yellow River</t>
+  </si>
+  <si>
+    <t>Caspian Sea</t>
+  </si>
+  <si>
+    <t>Continent</t>
   </si>
 </sst>
 </file>
@@ -136,9 +181,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,19 +467,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L54"/>
+  <dimension ref="A1:L63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="2" max="2" width="13.26953125" customWidth="1"/>
+    <col min="3" max="3" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -457,23 +510,23 @@
         <v>13</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -481,58 +534,128 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="C11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="F12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="C14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="C16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C24" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="E25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="E26" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Transferring to other computer
</commit_message>
<xml_diff>
--- a/map-data.xlsx
+++ b/map-data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Asia</t>
   </si>
@@ -138,6 +138,9 @@
   </si>
   <si>
     <t>Continent</t>
+  </si>
+  <si>
+    <t>Shanghai</t>
   </si>
 </sst>
 </file>
@@ -467,13 +470,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L63"/>
+  <dimension ref="A1:L64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K2" sqref="K2"/>
+      <selection pane="bottomRight" activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -630,32 +633,37 @@
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="E25" t="s">
-        <v>34</v>
+      <c r="C25" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.35">
       <c r="E26" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="E27" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A60" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>